<commit_message>
Edit servo_motor_control.ino to accomodate directive changes
</commit_message>
<xml_diff>
--- a/Lab 2/stepper table final.xlsx
+++ b/Lab 2/stepper table final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\Documents\Mechatronics\Lab 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cameronmesser/Documents/Mechatronics/Lab 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE40A2D9-1201-4609-A149-EC0E6E6F9DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8A363B-320E-AA45-82C0-E914E44D5016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stepper data" sheetId="1" r:id="rId1"/>
@@ -4854,9 +4854,9 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>5</v>
       </c>
@@ -4864,7 +4864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>5</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>5</v>
       </c>
@@ -4880,7 +4880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4904,7 +4904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4912,7 +4912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -4920,7 +4920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>5</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>5</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>5</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>5</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
@@ -4984,7 +4984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>5</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>5</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>5</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>5</v>
       </c>
@@ -5016,7 +5016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>5</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>5</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5</v>
       </c>
@@ -5040,7 +5040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>5</v>
       </c>
@@ -5048,7 +5048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>5</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>5</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>5</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>5</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>5</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>5</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>5</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>5</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>5</v>
       </c>
@@ -5120,7 +5120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>5</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>5</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>5</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>5</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>5</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>5</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>5</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>5</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>5</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>5</v>
       </c>
@@ -5200,7 +5200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>5</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>5</v>
       </c>
@@ -5216,7 +5216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>5</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>5</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>5</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>5</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>5</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>5</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>5</v>
       </c>
@@ -5272,7 +5272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>5</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>5</v>
       </c>
@@ -5288,7 +5288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>5</v>
       </c>
@@ -5296,7 +5296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>5</v>
       </c>
@@ -5304,7 +5304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>5</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>5</v>
       </c>
@@ -5320,7 +5320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>5</v>
       </c>
@@ -5328,7 +5328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>5</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>5</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>5</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>5</v>
       </c>
@@ -5360,7 +5360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>5</v>
       </c>
@@ -5368,7 +5368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>5</v>
       </c>
@@ -5376,7 +5376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>5</v>
       </c>
@@ -5384,7 +5384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>5</v>
       </c>
@@ -5392,7 +5392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>5</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>5</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>5</v>
       </c>
@@ -5416,7 +5416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>5</v>
       </c>
@@ -5424,7 +5424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>5</v>
       </c>
@@ -5432,7 +5432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>5</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>5</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>5</v>
       </c>
@@ -5456,7 +5456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>5</v>
       </c>
@@ -5464,7 +5464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>5</v>
       </c>
@@ -5472,7 +5472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>5</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>5</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>5</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>5</v>
       </c>
@@ -5504,7 +5504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>5</v>
       </c>
@@ -5512,7 +5512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>5</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>5</v>
       </c>
@@ -5528,7 +5528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>5</v>
       </c>
@@ -5536,7 +5536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>5</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>5</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>5</v>
       </c>
@@ -5560,7 +5560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>5</v>
       </c>
@@ -5568,7 +5568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>5</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>5</v>
       </c>
@@ -5584,7 +5584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>5</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>5</v>
       </c>
@@ -5600,7 +5600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>5</v>
       </c>
@@ -5608,7 +5608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>5</v>
       </c>
@@ -5616,7 +5616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>5</v>
       </c>
@@ -5624,7 +5624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>5</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>5</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>5</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>5</v>
       </c>
@@ -5656,7 +5656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>5</v>
       </c>
@@ -5664,7 +5664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>5</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>5</v>
       </c>
@@ -5680,7 +5680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>5</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>5</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>5</v>
       </c>
@@ -5704,7 +5704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>5</v>
       </c>
@@ -5712,7 +5712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>5</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>5</v>
       </c>
@@ -5728,7 +5728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>5</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>5</v>
       </c>
@@ -5744,7 +5744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>5</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>5</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>5</v>
       </c>
@@ -5768,7 +5768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>5</v>
       </c>
@@ -5776,7 +5776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>5</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>5</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>5</v>
       </c>
@@ -5800,7 +5800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>5</v>
       </c>
@@ -5808,7 +5808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>5</v>
       </c>
@@ -5816,7 +5816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>5</v>
       </c>
@@ -5824,7 +5824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>5</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>5</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>5</v>
       </c>
@@ -5848,7 +5848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>5</v>
       </c>
@@ -5856,7 +5856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>5</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>4.95</v>
       </c>
@@ -5872,7 +5872,7 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>4.5999999999999996</v>
       </c>
@@ -5880,7 +5880,7 @@
         <v>15.84</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>4.4400000000000004</v>
       </c>
@@ -5888,7 +5888,7 @@
         <v>22.29</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>4.4400000000000004</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>22.48</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>4.1399999999999997</v>
       </c>
@@ -5904,7 +5904,7 @@
         <v>34.409999999999997</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>4.13</v>
       </c>
@@ -5912,7 +5912,7 @@
         <v>34.6</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>3.89</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>44.57</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>3.87</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>45.16</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>3.54</v>
       </c>
@@ -5936,7 +5936,7 @@
         <v>58.26</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>3.21</v>
       </c>
@@ -5944,7 +5944,7 @@
         <v>71.75</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>2.78</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>88.76</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>2.4300000000000002</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>97.17</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>2.25</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>90.13</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>2.23</v>
       </c>
@@ -5976,7 +5976,7 @@
         <v>89.35</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>2.06</v>
       </c>
@@ -5984,7 +5984,7 @@
         <v>82.5</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>1.83</v>
       </c>
@@ -5992,7 +5992,7 @@
         <v>73.31</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>1.57</v>
       </c>
@@ -6000,7 +6000,7 @@
         <v>62.95</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>1.53</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>61.39</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>1.44</v>
       </c>
@@ -6016,7 +6016,7 @@
         <v>57.48</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>1.29</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>51.61</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>1.0900000000000001</v>
       </c>
@@ -6032,7 +6032,7 @@
         <v>43.6</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>1.08</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>43.01</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>0.96</v>
       </c>
@@ -6048,7 +6048,7 @@
         <v>38.51</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>0.75</v>
       </c>
@@ -6056,7 +6056,7 @@
         <v>30.11</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>0.44</v>
       </c>
@@ -6064,7 +6064,7 @@
         <v>17.79</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>0.37</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>14.66</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>0.22</v>
       </c>
@@ -6080,7 +6080,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>0.15</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>5.87</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>0</v>
       </c>
@@ -6096,7 +6096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>0</v>
       </c>
@@ -6104,7 +6104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>0</v>
       </c>
@@ -6112,7 +6112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>0</v>
       </c>
@@ -6120,7 +6120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>0</v>
       </c>
@@ -6128,7 +6128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>0</v>
       </c>
@@ -6136,7 +6136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>0</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>0</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>0</v>
       </c>
@@ -6160,7 +6160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>0</v>
       </c>
@@ -6168,7 +6168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>0</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>0</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>0</v>
       </c>
@@ -6192,7 +6192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>0</v>
       </c>
@@ -6200,7 +6200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>0</v>
       </c>
@@ -6208,7 +6208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>0</v>
       </c>
@@ -6216,7 +6216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>0</v>
       </c>
@@ -6224,7 +6224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>0</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>0</v>
       </c>
@@ -6240,7 +6240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>0</v>
       </c>
@@ -6248,7 +6248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>0</v>
       </c>
@@ -6256,7 +6256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>0</v>
       </c>
@@ -6264,7 +6264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>0</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>0</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>0</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>0</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>0</v>
       </c>
@@ -6304,7 +6304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>0</v>
       </c>
@@ -6312,7 +6312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>0</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>0</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>0</v>
       </c>
@@ -6336,7 +6336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>0</v>
       </c>
@@ -6344,7 +6344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>0</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>0</v>
       </c>
@@ -6360,7 +6360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>0</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>0</v>
       </c>
@@ -6376,7 +6376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>0</v>
       </c>
@@ -6384,7 +6384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>0</v>
       </c>
@@ -6392,7 +6392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>0</v>
       </c>
@@ -6400,7 +6400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>0</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>0</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>0</v>
       </c>
@@ -6424,7 +6424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>0</v>
       </c>
@@ -6432,7 +6432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>0</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>0</v>
       </c>
@@ -6448,7 +6448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>0</v>
       </c>
@@ -6456,7 +6456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>0</v>
       </c>
@@ -6464,7 +6464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>0</v>
       </c>
@@ -6472,7 +6472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>0</v>
       </c>
@@ -6480,7 +6480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>0</v>
       </c>
@@ -6488,7 +6488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>0</v>
       </c>
@@ -6496,7 +6496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>0</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>0</v>
       </c>
@@ -6512,7 +6512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>0</v>
       </c>
@@ -6520,7 +6520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>0</v>
       </c>
@@ -6528,7 +6528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>0</v>
       </c>
@@ -6536,7 +6536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>0.03</v>
       </c>
@@ -6544,7 +6544,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>0.46</v>
       </c>
@@ -6552,7 +6552,7 @@
         <v>18.38</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>0.52</v>
       </c>
@@ -6560,7 +6560,7 @@
         <v>20.92</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>0.89</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>35.58</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>1.0900000000000001</v>
       </c>
@@ -6576,7 +6576,7 @@
         <v>43.6</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>1.1200000000000001</v>
       </c>
@@ -6584,7 +6584,7 @@
         <v>44.77</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>1.38</v>
       </c>
@@ -6592,7 +6592,7 @@
         <v>55.13</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>1.48</v>
       </c>
@@ -6600,7 +6600,7 @@
         <v>59.24</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>1.82</v>
       </c>
@@ -6608,7 +6608,7 @@
         <v>72.73</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>2.08</v>
       </c>
@@ -6616,7 +6616,7 @@
         <v>83.28</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>2.11</v>
       </c>
@@ -6624,7 +6624,7 @@
         <v>84.46</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>2.21</v>
       </c>
@@ -6632,7 +6632,7 @@
         <v>88.56</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>2.2799999999999998</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>91.1</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>2.2799999999999998</v>
       </c>
@@ -6648,7 +6648,7 @@
         <v>91.3</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>2.39</v>
       </c>
@@ -6656,7 +6656,7 @@
         <v>95.6</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>2.54</v>
       </c>
@@ -6664,7 +6664,7 @@
         <v>98.53</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>2.72</v>
       </c>
@@ -6672,7 +6672,7 @@
         <v>91.1</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>2.74</v>
       </c>
@@ -6680,7 +6680,7 @@
         <v>90.52</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>2.81</v>
       </c>
@@ -6688,7 +6688,7 @@
         <v>87.78</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>3.05</v>
       </c>
@@ -6696,7 +6696,7 @@
         <v>77.81</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>3.2</v>
       </c>
@@ -6704,7 +6704,7 @@
         <v>72.14</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>3.25</v>
       </c>
@@ -6712,7 +6712,7 @@
         <v>70.19</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>3.3</v>
       </c>
@@ -6720,7 +6720,7 @@
         <v>67.84</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>3.32</v>
       </c>
@@ -6728,7 +6728,7 @@
         <v>67.25</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>3.4</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>64.13</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>3.6</v>
       </c>
@@ -6744,7 +6744,7 @@
         <v>56.11</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>3.67</v>
       </c>
@@ -6752,7 +6752,7 @@
         <v>53.37</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>3.85</v>
       </c>
@@ -6760,7 +6760,7 @@
         <v>45.94</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>3.89</v>
       </c>
@@ -6768,7 +6768,7 @@
         <v>44.38</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>3.97</v>
       </c>
@@ -6776,7 +6776,7 @@
         <v>41.06</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>4.03</v>
       </c>
@@ -6784,7 +6784,7 @@
         <v>38.909999999999997</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>4.18</v>
       </c>
@@ -6792,7 +6792,7 @@
         <v>32.840000000000003</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>4.22</v>
       </c>
@@ -6800,7 +6800,7 @@
         <v>31.09</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>4.0999999999999996</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>35.97</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>4.22</v>
       </c>
@@ -6816,7 +6816,7 @@
         <v>31.09</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>4.5999999999999996</v>
       </c>
@@ -6824,7 +6824,7 @@
         <v>15.84</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>4.6500000000000004</v>
       </c>
@@ -6832,7 +6832,7 @@
         <v>13.88</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>4.71</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v>11.73</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>4.88</v>
       </c>
@@ -6848,7 +6848,7 @@
         <v>4.6900000000000004</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>4.95</v>
       </c>
@@ -6856,7 +6856,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>5</v>
       </c>
@@ -6864,7 +6864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>5</v>
       </c>
@@ -6872,7 +6872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>5</v>
       </c>
@@ -6880,7 +6880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>5</v>
       </c>
@@ -6888,7 +6888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>5</v>
       </c>
@@ -6896,7 +6896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>5</v>
       </c>
@@ -6904,7 +6904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>5</v>
       </c>
@@ -6912,7 +6912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>5</v>
       </c>
@@ -6920,7 +6920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>5</v>
       </c>
@@ -6928,7 +6928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>5</v>
       </c>
@@ -6936,7 +6936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>5</v>
       </c>
@@ -6944,7 +6944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>5</v>
       </c>
@@ -6952,7 +6952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>5</v>
       </c>
@@ -6960,7 +6960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>5</v>
       </c>
@@ -6968,7 +6968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>5</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>5</v>
       </c>
@@ -6984,7 +6984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>5</v>
       </c>
@@ -6992,7 +6992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>5</v>
       </c>
@@ -7000,7 +7000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>5</v>
       </c>
@@ -7008,7 +7008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>5</v>
       </c>
@@ -7016,7 +7016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>5</v>
       </c>
@@ -7024,7 +7024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>5</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>5</v>
       </c>
@@ -7040,7 +7040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>5</v>
       </c>
@@ -7048,7 +7048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>5</v>
       </c>
@@ -7056,7 +7056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>5</v>
       </c>
@@ -7064,7 +7064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>5</v>
       </c>
@@ -7072,7 +7072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>5</v>
       </c>
@@ -7080,7 +7080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>5</v>
       </c>
@@ -7088,7 +7088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>5</v>
       </c>
@@ -7096,7 +7096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>5</v>
       </c>
@@ -7104,7 +7104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>5</v>
       </c>
@@ -7112,7 +7112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>5</v>
       </c>
@@ -7120,7 +7120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>5</v>
       </c>
@@ -7128,7 +7128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>5</v>
       </c>
@@ -7136,7 +7136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>5</v>
       </c>
@@ -7144,7 +7144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>5</v>
       </c>
@@ -7152,7 +7152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>5</v>
       </c>
@@ -7160,7 +7160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>5</v>
       </c>
@@ -7168,7 +7168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>5</v>
       </c>
@@ -7176,7 +7176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>5</v>
       </c>
@@ -7184,7 +7184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>5</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>5</v>
       </c>
@@ -7200,7 +7200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>5</v>
       </c>
@@ -7208,7 +7208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>5</v>
       </c>
@@ -7216,7 +7216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>5</v>
       </c>
@@ -7224,7 +7224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>5</v>
       </c>
@@ -7232,7 +7232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>5</v>
       </c>
@@ -7240,7 +7240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>5</v>
       </c>
@@ -7248,7 +7248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>5</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>5</v>
       </c>
@@ -7264,7 +7264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>5</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>5</v>
       </c>
@@ -7280,7 +7280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>5</v>
       </c>
@@ -7288,7 +7288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>5</v>
       </c>
@@ -7296,7 +7296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>5</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>5</v>
       </c>
@@ -7312,7 +7312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>5</v>
       </c>
@@ -7320,7 +7320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>5</v>
       </c>
@@ -7328,7 +7328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>5</v>
       </c>
@@ -7336,7 +7336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>5</v>
       </c>
@@ -7344,7 +7344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>5</v>
       </c>
@@ -7352,7 +7352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>4.9800000000000004</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>4.49</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>20.329999999999998</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>4.46</v>
       </c>
@@ -7376,7 +7376,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>4.34</v>
       </c>
@@ -7384,7 +7384,7 @@
         <v>26.59</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>4.26</v>
       </c>
@@ -7392,7 +7392,7 @@
         <v>29.72</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>3.86</v>
       </c>
@@ -7400,7 +7400,7 @@
         <v>45.55</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>3.85</v>
       </c>
@@ -7408,7 +7408,7 @@
         <v>45.94</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>3.75</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v>50.05</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>3.39</v>
       </c>
@@ -7424,7 +7424,7 @@
         <v>64.319999999999993</v>
       </c>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>3.28</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>68.62</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>3.13</v>
       </c>
@@ -7440,7 +7440,7 @@
         <v>74.88</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>2.94</v>
       </c>
@@ -7448,7 +7448,7 @@
         <v>82.5</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>2.65</v>
       </c>
@@ -7456,7 +7456,7 @@
         <v>94.04</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>2.2400000000000002</v>
       </c>
@@ -7464,7 +7464,7 @@
         <v>89.54</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>2.14</v>
       </c>
@@ -7472,7 +7472,7 @@
         <v>85.63</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>2.0099999999999998</v>
       </c>
@@ -7480,7 +7480,7 @@
         <v>80.55</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>1.74</v>
       </c>
@@ -7488,7 +7488,7 @@
         <v>69.599999999999994</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>1.6</v>
       </c>
@@ -7496,7 +7496,7 @@
         <v>64.13</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>1.34</v>
       </c>
@@ -7504,7 +7504,7 @@
         <v>53.57</v>
       </c>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>1.17</v>
       </c>
@@ -7512,7 +7512,7 @@
         <v>46.73</v>
       </c>
     </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>0.94</v>
       </c>
@@ -7520,7 +7520,7 @@
         <v>37.729999999999997</v>
       </c>
     </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>0.88</v>
       </c>
@@ -7528,7 +7528,7 @@
         <v>35.39</v>
       </c>
     </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>0.55000000000000004</v>
       </c>
@@ -7536,7 +7536,7 @@
         <v>22.09</v>
       </c>
     </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>0.41</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>16.23</v>
       </c>
     </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>0.23</v>
       </c>
@@ -7552,7 +7552,7 @@
         <v>9.19</v>
       </c>
     </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>0.22</v>
       </c>
@@ -7560,7 +7560,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>0</v>
       </c>
@@ -7568,7 +7568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>0</v>
       </c>
@@ -7576,7 +7576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>0</v>
       </c>
@@ -7584,7 +7584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>0</v>
       </c>
@@ -7592,7 +7592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>0</v>
       </c>
@@ -7600,7 +7600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>0</v>
       </c>
@@ -7608,7 +7608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>0</v>
       </c>
@@ -7616,7 +7616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>0</v>
       </c>
@@ -7624,7 +7624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>0</v>
       </c>
@@ -7632,7 +7632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A348">
         <v>0</v>
       </c>
@@ -7640,7 +7640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>0</v>
       </c>
@@ -7648,7 +7648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A350">
         <v>0</v>
       </c>
@@ -7656,7 +7656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A351">
         <v>0</v>
       </c>
@@ -7664,7 +7664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A352">
         <v>0</v>
       </c>
@@ -7672,7 +7672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A353">
         <v>0</v>
       </c>
@@ -7680,7 +7680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A354">
         <v>0</v>
       </c>
@@ -7688,7 +7688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A355">
         <v>0</v>
       </c>
@@ -7696,7 +7696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A356">
         <v>0</v>
       </c>
@@ -7704,7 +7704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A357">
         <v>0</v>
       </c>
@@ -7712,7 +7712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A358">
         <v>0</v>
       </c>
@@ -7720,7 +7720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A359">
         <v>0</v>
       </c>
@@ -7728,7 +7728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360">
         <v>0</v>
       </c>
@@ -7736,7 +7736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A361">
         <v>0</v>
       </c>
@@ -7744,7 +7744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A362">
         <v>0</v>
       </c>
@@ -7752,7 +7752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A363">
         <v>0</v>
       </c>
@@ -7760,7 +7760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A364">
         <v>0</v>
       </c>
@@ -7768,7 +7768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A365">
         <v>0</v>
       </c>
@@ -7776,7 +7776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A366">
         <v>0</v>
       </c>
@@ -7784,7 +7784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A367">
         <v>0</v>
       </c>
@@ -7792,7 +7792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A368">
         <v>0</v>
       </c>
@@ -7800,7 +7800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A369">
         <v>0</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A370">
         <v>0</v>
       </c>
@@ -7816,7 +7816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A371">
         <v>0</v>
       </c>
@@ -7824,7 +7824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A372">
         <v>0</v>
       </c>
@@ -7832,7 +7832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A373">
         <v>0</v>
       </c>
@@ -7840,7 +7840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A374">
         <v>0</v>
       </c>
@@ -7848,7 +7848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A375">
         <v>0</v>
       </c>
@@ -7856,7 +7856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376">
         <v>0</v>
       </c>
@@ -7864,7 +7864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A377">
         <v>0</v>
       </c>
@@ -7872,7 +7872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A378">
         <v>0</v>
       </c>
@@ -7880,7 +7880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A379">
         <v>0</v>
       </c>
@@ -7888,7 +7888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A380">
         <v>0</v>
       </c>
@@ -7896,7 +7896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A381">
         <v>0</v>
       </c>
@@ -7904,7 +7904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A382">
         <v>0</v>
       </c>
@@ -7912,7 +7912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A383">
         <v>0</v>
       </c>
@@ -7920,7 +7920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A384">
         <v>0</v>
       </c>
@@ -7928,7 +7928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>0</v>
       </c>
@@ -7936,7 +7936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A386">
         <v>0</v>
       </c>
@@ -7944,7 +7944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A387">
         <v>0</v>
       </c>
@@ -7952,7 +7952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A388">
         <v>0</v>
       </c>
@@ -7960,7 +7960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A389">
         <v>0</v>
       </c>
@@ -7968,7 +7968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A390">
         <v>0</v>
       </c>
@@ -7976,7 +7976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A391">
         <v>0</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A392">
         <v>0</v>
       </c>
@@ -7992,7 +7992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A393">
         <v>0</v>
       </c>
@@ -8000,7 +8000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A394">
         <v>0</v>
       </c>
@@ -8008,7 +8008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A395">
         <v>0</v>
       </c>
@@ -8016,7 +8016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A396">
         <v>0</v>
       </c>
@@ -8024,7 +8024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A397">
         <v>0</v>
       </c>
@@ -8032,7 +8032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A398">
         <v>0</v>
       </c>
@@ -8040,7 +8040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A399">
         <v>0</v>
       </c>
@@ -8048,7 +8048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A400">
         <v>0</v>
       </c>
@@ -8056,7 +8056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A401">
         <v>0</v>
       </c>
@@ -8064,7 +8064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A402">
         <v>0</v>
       </c>
@@ -8072,7 +8072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A403">
         <v>0</v>
       </c>
@@ -8080,7 +8080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A404">
         <v>0</v>
       </c>
@@ -8088,7 +8088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A405">
         <v>0</v>
       </c>
@@ -8096,7 +8096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A406">
         <v>0</v>
       </c>
@@ -8104,7 +8104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A407">
         <v>0</v>
       </c>
@@ -8112,7 +8112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A408">
         <v>0</v>
       </c>
@@ -8120,7 +8120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A409">
         <v>0</v>
       </c>
@@ -8128,7 +8128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A410">
         <v>0</v>
       </c>
@@ -8136,7 +8136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A411">
         <v>0</v>
       </c>
@@ -8144,7 +8144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A412">
         <v>0</v>
       </c>
@@ -8152,7 +8152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A413">
         <v>0</v>
       </c>
@@ -8160,7 +8160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A414">
         <v>0</v>
       </c>
@@ -8168,7 +8168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A415">
         <v>0</v>
       </c>
@@ -8176,7 +8176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A416">
         <v>0</v>
       </c>
@@ -8184,7 +8184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A417">
         <v>0</v>
       </c>
@@ -8192,7 +8192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A418">
         <v>0</v>
       </c>
@@ -8200,7 +8200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A419">
         <v>0</v>
       </c>
@@ -8208,7 +8208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A420">
         <v>0</v>
       </c>
@@ -8216,7 +8216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A421">
         <v>0</v>
       </c>
@@ -8224,7 +8224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A422">
         <v>0</v>
       </c>
@@ -8232,7 +8232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A423">
         <v>0</v>
       </c>
@@ -8240,7 +8240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A424">
         <v>0</v>
       </c>
@@ -8248,7 +8248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A425">
         <v>0</v>
       </c>
@@ -8256,7 +8256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A426">
         <v>0</v>
       </c>
@@ -8264,7 +8264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A427">
         <v>0</v>
       </c>
@@ -8272,7 +8272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A428">
         <v>0</v>
       </c>
@@ -8280,7 +8280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A429">
         <v>0</v>
       </c>
@@ -8288,7 +8288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A430">
         <v>0</v>
       </c>
@@ -8296,7 +8296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A431">
         <v>0</v>
       </c>
@@ -8304,7 +8304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A432">
         <v>0</v>
       </c>
@@ -8312,7 +8312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A433">
         <v>0</v>
       </c>
@@ -8320,7 +8320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A434">
         <v>0</v>
       </c>
@@ -8328,7 +8328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A435">
         <v>0</v>
       </c>
@@ -8336,7 +8336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A436">
         <v>0</v>
       </c>
@@ -8344,7 +8344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A437">
         <v>0</v>
       </c>
@@ -8352,7 +8352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A438">
         <v>0</v>
       </c>
@@ -8360,7 +8360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A439">
         <v>0</v>
       </c>
@@ -8368,7 +8368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A440">
         <v>0</v>
       </c>
@@ -8376,7 +8376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A441">
         <v>0</v>
       </c>
@@ -8384,7 +8384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A442">
         <v>0</v>
       </c>
@@ -8392,7 +8392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A443">
         <v>0</v>
       </c>
@@ -8400,7 +8400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A444">
         <v>0</v>
       </c>
@@ -8408,7 +8408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A445">
         <v>0</v>
       </c>
@@ -8416,7 +8416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A446">
         <v>0</v>
       </c>
@@ -8424,7 +8424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A447">
         <v>0</v>
       </c>
@@ -8432,7 +8432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A448">
         <v>0</v>
       </c>
@@ -8440,7 +8440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A449">
         <v>0</v>
       </c>
@@ -8448,7 +8448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A450">
         <v>0</v>
       </c>
@@ -8456,7 +8456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A451">
         <v>0</v>
       </c>
@@ -8464,7 +8464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A452">
         <v>0</v>
       </c>
@@ -8472,7 +8472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A453">
         <v>0</v>
       </c>
@@ -8480,7 +8480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A454">
         <v>0</v>
       </c>
@@ -8488,7 +8488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A455">
         <v>0</v>
       </c>
@@ -8496,7 +8496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A456">
         <v>0</v>
       </c>
@@ -8504,7 +8504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A457">
         <v>0</v>
       </c>
@@ -8512,7 +8512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A458">
         <v>0</v>
       </c>
@@ -8520,7 +8520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A459">
         <v>0</v>
       </c>
@@ -8528,7 +8528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A460">
         <v>0</v>
       </c>
@@ -8536,7 +8536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A461">
         <v>0</v>
       </c>
@@ -8544,7 +8544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A462">
         <v>0</v>
       </c>
@@ -8552,7 +8552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A463">
         <v>0</v>
       </c>
@@ -8560,7 +8560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A464">
         <v>0</v>
       </c>
@@ -8568,7 +8568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A465">
         <v>0</v>
       </c>
@@ -8576,7 +8576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A466">
         <v>0</v>
       </c>
@@ -8584,7 +8584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A467">
         <v>0</v>
       </c>
@@ -8592,7 +8592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A468">
         <v>0</v>
       </c>
@@ -8600,7 +8600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A469">
         <v>0</v>
       </c>
@@ -8608,7 +8608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A470">
         <v>0</v>
       </c>
@@ -8616,7 +8616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A471">
         <v>0</v>
       </c>
@@ -8624,7 +8624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A472">
         <v>0</v>
       </c>
@@ -8632,7 +8632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A473">
         <v>0</v>
       </c>
@@ -8640,7 +8640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A474">
         <v>0</v>
       </c>
@@ -8648,7 +8648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A475">
         <v>0</v>
       </c>
@@ -8656,7 +8656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A476">
         <v>0</v>
       </c>
@@ -8664,7 +8664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A477">
         <v>0</v>
       </c>
@@ -8672,7 +8672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A478">
         <v>0</v>
       </c>
@@ -8680,7 +8680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A479">
         <v>0</v>
       </c>
@@ -8688,7 +8688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A480">
         <v>0</v>
       </c>
@@ -8696,7 +8696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="481" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A481">
         <v>0</v>
       </c>
@@ -8704,7 +8704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A482">
         <v>0</v>
       </c>
@@ -8712,7 +8712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A483">
         <v>0</v>
       </c>
@@ -8720,7 +8720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="484" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A484">
         <v>0</v>
       </c>
@@ -8728,7 +8728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A485">
         <v>0</v>
       </c>
@@ -8736,7 +8736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="486" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A486">
         <v>0</v>
       </c>
@@ -8744,7 +8744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="487" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A487">
         <v>0</v>
       </c>
@@ -8752,7 +8752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="488" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A488">
         <v>0</v>
       </c>
@@ -8760,7 +8760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="489" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A489">
         <v>0</v>
       </c>
@@ -8768,7 +8768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="490" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A490">
         <v>0</v>
       </c>
@@ -8776,7 +8776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="491" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A491">
         <v>0</v>
       </c>
@@ -8784,7 +8784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="492" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A492">
         <v>0</v>
       </c>
@@ -8792,7 +8792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="493" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A493">
         <v>0</v>
       </c>
@@ -8800,7 +8800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="494" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A494">
         <v>0</v>
       </c>

</xml_diff>